<commit_message>
Improve Excel file parsing and template generation.  Add a simpler, more robust template download option to handle various Excel file formats.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 9721d37c-4240-4a5a-982a-dc1cc1c5c3b7
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/99e565d9-defe-4b43-9370-4d17ce50e7be/5eafa977-be94-4032-aaf0-28bbdaec7f0c.jpg
</commit_message>
<xml_diff>
--- a/ultra-simple-template.xlsx
+++ b/ultra-simple-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Simple Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -402,10 +402,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="70.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>example-file-123.mp3</v>
+        <v>agent-261-17027502083-444.mp3</v>
       </c>
       <c r="B2" t="str">
         <v>english</v>

</xml_diff>